<commit_message>
Backup QR Scanner data - 10/05/2025, 3:16:16 AM
</commit_message>
<xml_diff>
--- a/backups/Checklist_Biochemistry_2025-05-09T22-59-58.xlsx
+++ b/backups/Checklist_Biochemistry_2025-05-09T22-59-58.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -453,9 +453,26 @@
         <v>240252</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>885</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Biochemistry</v>
+      </c>
+      <c r="C4" t="str">
+        <v>10/05/2025</v>
+      </c>
+      <c r="D4" t="str">
+        <v>03:16:00</v>
+      </c>
+      <c r="E4" t="str">
+        <v>885</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>